<commit_message>
MM Switches and BOM
</commit_message>
<xml_diff>
--- a/GERBER/BOM.xlsx
+++ b/GERBER/BOM.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="J0" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="F0" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="MM" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="135">
   <si>
     <t xml:space="preserve">J0</t>
   </si>
@@ -279,15 +280,163 @@
   </si>
   <si>
     <t xml:space="preserve">CR0603-FX-4701ELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWITCHES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW_SEL/MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100DP6T1B1M2QE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW_BRIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100SP1T1B1M2QEH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2, C13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECH-U1C182JX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCP1A106M8R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6, C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VJ0603A471GXXCW1BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8, C12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECH-U1C473GX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMBF5457</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3, R9, R10, R12, R14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4, R16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5, R13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6, R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV16AF-20-15S1-C1M-LA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV16AF-20-15S1-A250K-LA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D\-MMM"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -354,7 +503,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -364,6 +513,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -387,18 +552,18 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,17 +1246,17 @@
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8520408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,6 +2119,738 @@
       <c r="H42" s="0" t="n">
         <f aca="false">F42*25</f>
         <v>2.95</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="18.4744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">F3*G3</f>
+        <v>22.84</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">F4*G4</f>
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <f aca="false">B10*2</f>
+        <v>2</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">F10*G10</f>
+        <v>1.254</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <f aca="false">B11*2</f>
+        <v>4</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.331</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <f aca="false">F11*G11</f>
+        <v>1.324</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <f aca="false">B12*2</f>
+        <v>2</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0.791</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">F12*G12</f>
+        <v>1.582</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <f aca="false">B13*2</f>
+        <v>2</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">F13*G13</f>
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">B14*2</f>
+        <v>2</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0.549</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">F14*G14</f>
+        <v>1.098</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">B15*2</f>
+        <v>4</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0.657</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">F15*G15</f>
+        <v>2.628</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <f aca="false">B16*2</f>
+        <v>2</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <f aca="false">F16*G16</f>
+        <v>0.268</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <f aca="false">B17*2</f>
+        <v>4</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">F17*G17</f>
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <f aca="false">B18*2</f>
+        <v>2</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">F18*G18</f>
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <f aca="false">B19*2</f>
+        <v>2</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0.253</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">F19*G19</f>
+        <v>0.506</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <f aca="false">B20*2</f>
+        <v>2</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <f aca="false">F20*G20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <f aca="false">B21*2</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">F21*G21</f>
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <f aca="false">B22*2</f>
+        <v>2</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <f aca="false">F22*G22</f>
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <f aca="false">B23*2</f>
+        <v>10</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <f aca="false">F23*G23</f>
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <f aca="false">B24*2</f>
+        <v>4</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <f aca="false">F24*G24</f>
+        <v>0.076</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <f aca="false">B25*2</f>
+        <v>4</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <f aca="false">F25*G25</f>
+        <v>0.076</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <f aca="false">B26*2</f>
+        <v>4</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">F26*G26</f>
+        <v>0.076</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <f aca="false">B27*2</f>
+        <v>2</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">F27*G27</f>
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">B28*2</f>
+        <v>2</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <f aca="false">F28*G28</f>
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <f aca="false">B29*2</f>
+        <v>2</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">F29*G29</f>
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <f aca="false">B30*2</f>
+        <v>2</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">F30*G30</f>
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <f aca="false">B31*2</f>
+        <v>2</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <f aca="false">F31*G31</f>
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <f aca="false">B34*2</f>
+        <v>2</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <f aca="false">F34*G34</f>
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">B36*2</f>
+        <v>6</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0.616</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <f aca="false">F36*G36</f>
+        <v>3.696</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <f aca="false">B37*2</f>
+        <v>4</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <f aca="false">F37*G37</f>
+        <v>5.96</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="0" t="n">
+        <f aca="false">SUM(H3:H37)</f>
+        <v>62.516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM Work prior to sending Gerbers
</commit_message>
<xml_diff>
--- a/GERBER/BOM.xlsx
+++ b/GERBER/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="J0" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="171">
   <si>
     <t xml:space="preserve">J0</t>
   </si>
@@ -436,37 +436,119 @@
     <t xml:space="preserve">RV16AF-20-15S1-A250K-LA</t>
   </si>
   <si>
-    <t xml:space="preserve">ECH-U1C182JX5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.022u</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECH-U1C223JX5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CR0603-FX-1000HLF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CR0603-FX-2003ELF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CR0603-FX-4703ELF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RV</t>
+    <t xml:space="preserve">TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RATING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOOTPRINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PART</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QTY 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QTY BEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COST1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COST10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COST50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHEETS DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CERMAIC C0G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VJ0603A271JXACW1BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FILM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCA0805C104M-J2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECH-U1C103GX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANTALUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAJR105K020YNJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CERAMIC X5R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMK316ABJ106KD-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PINS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERM BLOCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP MOUSER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALPHA CONCENTRIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A100k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B50k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D\-MMM"/>
     <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="[$$-C09]#,##0.00;[RED]\-[$$-C09]#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -487,6 +569,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -531,7 +618,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -560,6 +647,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -580,15 +675,18 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,11 +1375,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2164,16 +2262,16 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2953,732 +3051,464 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6020408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.3673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="0" t="n">
-        <v>0.791</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <f aca="false">F1*B1</f>
-        <v>2.373</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">B2*2</f>
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="J2" s="0" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>0.097</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">B3*2</f>
+        <v>2</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.697</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0.697</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0.627</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <f aca="false">F2*B2</f>
-        <v>5.016</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0.978</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <f aca="false">F3*B3</f>
-        <v>0.978</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="D4" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="0" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <f aca="false">F4*B4</f>
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>152</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">B4*2</f>
+        <v>4</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.495</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0.495</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">B5*2</f>
+        <v>4</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.261</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0.261</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="0" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <f aca="false">F5*B5</f>
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="D6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="0" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <f aca="false">F6*B6</f>
-        <v>0.096</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>155</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">B6*2</f>
+        <v>4</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.685</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0.685</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>0.331</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <f aca="false">F7*B7</f>
-        <v>1.655</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>1.89</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <f aca="false">F8*B8</f>
-        <v>1.89</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>158</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">B7*2</f>
+        <v>4</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.567</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.271</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0.271</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="B9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>138</v>
+        <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>0.697</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <f aca="false">F9*B9</f>
-        <v>1.394</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>0.431</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">F10*B10</f>
-        <v>0.431</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>160</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>161</v>
+      </c>
       <c r="B11" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <f aca="false">F11*B11</f>
-        <v>0.288</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="0" t="n">
-        <v>0.134</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <f aca="false">F12*B12</f>
-        <v>0.134</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="0" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <f aca="false">F13*B13</f>
-        <v>1.15</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0.657</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">F14*B14</f>
-        <v>3.942</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>21</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C15" s="0" t="s">
+        <v>162</v>
+      </c>
       <c r="D15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>0.253</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">F15*B15</f>
-        <v>0.759</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <f aca="false">F16*B16</f>
-        <v>0.038</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="B18" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <f aca="false">F17*B17</f>
-        <v>0.084</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <f aca="false">F18*B18</f>
-        <v>0.114</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C19" s="0" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <f aca="false">F19*B19</f>
-        <v>0.114</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <f aca="false">F20*B20</f>
-        <v>0.019</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="0" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <f aca="false">F21*B21</f>
-        <v>0.019</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <f aca="false">F22*B22</f>
-        <v>0.133</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>0.009</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <f aca="false">F23*B23</f>
-        <v>0.045</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <f aca="false">F24*B24</f>
-        <v>0.076</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <f aca="false">F25*B25</f>
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <f aca="false">F26*B26</f>
-        <v>0.019</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <v>0.009</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <f aca="false">F27*B27</f>
-        <v>0.018</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <f aca="false">F28*B28</f>
-        <v>0.038</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F29" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G29" s="0" t="n">
-        <f aca="false">F29*B29</f>
-        <v>0.019</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="0" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="G30" s="0" t="n">
-        <f aca="false">F30*B30</f>
-        <v>0.038</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
-      <c r="B31" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="G31" s="0" t="n">
-        <f aca="false">F31*B31</f>
-        <v>0.024</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="4" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="0" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="G32" s="0" t="n">
-        <f aca="false">F32*B32</f>
-        <v>3.81</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="G33" s="0" t="n">
-        <f aca="false">F33*B33</f>
-        <v>2.16</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="G34" s="0" t="n">
-        <f aca="false">F34*B34</f>
-        <v>2.16</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <v>0.616</v>
-      </c>
-      <c r="G35" s="0" t="n">
-        <f aca="false">F35*B35</f>
-        <v>6.16</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <v>1.49</v>
-      </c>
-      <c r="G36" s="0" t="n">
-        <f aca="false">F36*B36</f>
-        <v>5.96</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F37" s="0" t="n">
-        <v>5.71</v>
-      </c>
-      <c r="G37" s="0" t="n">
-        <f aca="false">F37*B37</f>
-        <v>11.42</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="G38" s="0" t="n">
-        <f aca="false">F38*B38</f>
-        <v>2.83</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G39" s="0" t="n">
-        <f aca="false">SUM(G1:G38)</f>
-        <v>59.054</v>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>